<commit_message>
LMS8 upload and results
</commit_message>
<xml_diff>
--- a/results/LMS2_storage type.xlsx
+++ b/results/LMS2_storage type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://001gc-my.sharepoint.com/personal/chih-yu_hung_agr_gc_ca/Documents/AAFC/Project 11_Can Farm survey/FMS/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_0164ECA346742EF02135BF3869F10D5359FFB48D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF192C00-2AED-4159-AA50-E5A41EE478AC}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_24A4CFA72FF469C0AF34BF4E01029FC6520BB47C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2EED1F5-EEB9-4C83-9C63-E07FFEC77487}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,19 +520,19 @@
         <v>2017</v>
       </c>
       <c r="F2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="G2" s="1">
         <v>2017</v>
       </c>
       <c r="H2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="I2" s="1">
         <v>2017</v>
       </c>
       <c r="J2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="K2" s="1">
         <v>2017</v>
@@ -541,19 +541,19 @@
         <v>2022</v>
       </c>
       <c r="M2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="N2" s="1">
         <v>2022</v>
       </c>
       <c r="O2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="P2" s="1">
         <v>2022</v>
       </c>
       <c r="Q2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="R2" s="1">
         <v>2022</v>
@@ -576,40 +576,40 @@
         <v>17.600000000000001</v>
       </c>
       <c r="F3" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G3" s="1">
         <v>162.1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
+        <v>172</v>
+      </c>
+      <c r="I3" s="1">
         <v>8.5</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="K3" s="1">
         <v>16.399999999999999</v>
       </c>
-      <c r="I3" s="1">
+      <c r="L3" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M3" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J3" s="1">
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
         <v>2.2000000000000002</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="L3" s="1">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="M3" s="1">
-        <v>172</v>
-      </c>
-      <c r="N3" s="1">
-        <v>13.4</v>
-      </c>
-      <c r="O3" s="1">
-        <v>4.0999999999999996</v>
       </c>
       <c r="P3" s="1">
         <v>7.6</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
@@ -632,40 +632,40 @@
         <v>15.5</v>
       </c>
       <c r="F4" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="G4" s="1">
         <v>61.3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
+        <v>47.1</v>
+      </c>
+      <c r="I4" s="1">
         <v>44.1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
+        <v>45.5</v>
+      </c>
+      <c r="K4" s="1">
         <v>17.7</v>
       </c>
-      <c r="I4" s="1">
+      <c r="L4" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="M4" s="1">
         <v>59.2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="1">
+        <v>47.9</v>
+      </c>
+      <c r="O4" s="1">
         <v>27.5</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L4" s="1">
-        <v>13.2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>47.1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>45.5</v>
-      </c>
-      <c r="O4" s="1">
-        <v>13.6</v>
       </c>
       <c r="P4" s="1">
         <v>22.7</v>
       </c>
       <c r="Q4" s="1">
-        <v>47.9</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
@@ -688,40 +688,40 @@
         <v>4</v>
       </c>
       <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>45.7</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
       <c r="H5" s="1">
+        <v>44.4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6</v>
+      </c>
+      <c r="K5" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>5.0999999999999996</v>
-      </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="M5" s="1">
-        <v>44.4</v>
+        <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="O5" s="1">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>4.3</v>
       </c>
       <c r="Q5" s="1">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
@@ -744,40 +744,40 @@
         <v>5.6</v>
       </c>
       <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
         <v>57.1</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>12.4</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
         <v>6.9</v>
       </c>
-      <c r="I6" s="1">
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>13.7</v>
       </c>
-      <c r="J6" s="1">
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
         <v>7.5</v>
       </c>
-      <c r="K6" s="1">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
         <v>3.6</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
@@ -800,40 +800,40 @@
         <v>8</v>
       </c>
       <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
         <v>40.4</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
         <v>24</v>
       </c>
-      <c r="H7" s="1">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
         <v>6.1</v>
       </c>
-      <c r="I7" s="1">
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
         <v>21.2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
         <v>25.5</v>
       </c>
-      <c r="K7" s="1">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
         <v>10.199999999999999</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
@@ -856,40 +856,40 @@
         <v>41.4</v>
       </c>
       <c r="F8" s="1">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1">
         <v>424.9</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
+        <v>488.8</v>
+      </c>
+      <c r="I8" s="1">
         <v>342.2</v>
       </c>
-      <c r="H8" s="1">
+      <c r="J8" s="1">
+        <v>311.7</v>
+      </c>
+      <c r="K8" s="1">
         <v>234</v>
       </c>
-      <c r="I8" s="1">
+      <c r="L8" s="1">
+        <v>139.5</v>
+      </c>
+      <c r="M8" s="1">
         <v>615.20000000000005</v>
       </c>
-      <c r="J8" s="1">
+      <c r="N8" s="1">
+        <v>688</v>
+      </c>
+      <c r="O8" s="1">
         <v>193</v>
-      </c>
-      <c r="K8" s="1">
-        <v>62.1</v>
-      </c>
-      <c r="L8" s="1">
-        <v>23</v>
-      </c>
-      <c r="M8" s="1">
-        <v>488.8</v>
-      </c>
-      <c r="N8" s="1">
-        <v>311.7</v>
-      </c>
-      <c r="O8" s="1">
-        <v>139.5</v>
       </c>
       <c r="P8" s="1">
         <v>174.7</v>
       </c>
       <c r="Q8" s="1">
-        <v>688</v>
+        <v>62.1</v>
       </c>
       <c r="R8" s="1">
         <v>24.4</v>
@@ -912,40 +912,40 @@
         <v>84.9</v>
       </c>
       <c r="F9" s="1">
+        <v>59.3</v>
+      </c>
+      <c r="G9" s="1">
         <v>573.5</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
+        <v>400.1</v>
+      </c>
+      <c r="I9" s="1">
         <v>38.200000000000003</v>
       </c>
-      <c r="H9" s="1">
+      <c r="J9" s="1">
+        <v>133.19999999999999</v>
+      </c>
+      <c r="K9" s="1">
         <v>438.8</v>
       </c>
-      <c r="I9" s="1">
+      <c r="L9" s="1">
+        <v>562.29999999999995</v>
+      </c>
+      <c r="M9" s="1">
         <v>1687.4</v>
       </c>
-      <c r="J9" s="1">
+      <c r="N9" s="1">
+        <v>1443.7</v>
+      </c>
+      <c r="O9" s="1">
         <v>16.899999999999999</v>
-      </c>
-      <c r="K9" s="1">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="L9" s="1">
-        <v>59.3</v>
-      </c>
-      <c r="M9" s="1">
-        <v>400.1</v>
-      </c>
-      <c r="N9" s="1">
-        <v>133.19999999999999</v>
-      </c>
-      <c r="O9" s="1">
-        <v>562.29999999999995</v>
       </c>
       <c r="P9" s="1">
         <v>63.5</v>
       </c>
       <c r="Q9" s="1">
-        <v>1443.7</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="R9" s="1">
         <v>38.799999999999997</v>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
@@ -989,10 +989,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="O10" s="1">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="R10" s="1">
         <v>0</v>
@@ -1024,40 +1024,40 @@
         <v>177</v>
       </c>
       <c r="F11" s="1">
+        <v>104.3</v>
+      </c>
+      <c r="G11" s="1">
         <v>1365</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
+        <v>1193.4000000000001</v>
+      </c>
+      <c r="I11" s="1">
         <v>469.4</v>
       </c>
-      <c r="H11" s="1">
+      <c r="J11" s="1">
+        <v>509.8</v>
+      </c>
+      <c r="K11" s="1">
         <v>722.1</v>
       </c>
-      <c r="I11" s="1">
+      <c r="L11" s="1">
+        <v>725.1</v>
+      </c>
+      <c r="M11" s="1">
         <v>2401.6</v>
       </c>
-      <c r="J11" s="1">
+      <c r="N11" s="1">
+        <v>2185.6999999999998</v>
+      </c>
+      <c r="O11" s="1">
         <v>272.60000000000002</v>
-      </c>
-      <c r="K11" s="1">
-        <v>152.9</v>
-      </c>
-      <c r="L11" s="1">
-        <v>104.3</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1193.4000000000001</v>
-      </c>
-      <c r="N11" s="1">
-        <v>509.8</v>
-      </c>
-      <c r="O11" s="1">
-        <v>725.1</v>
       </c>
       <c r="P11" s="1">
         <v>272.8</v>
       </c>
       <c r="Q11" s="1">
-        <v>2185.6999999999998</v>
+        <v>152.9</v>
       </c>
       <c r="R11" s="1">
         <v>63.2</v>
@@ -1080,19 +1080,19 @@
         <v>2017</v>
       </c>
       <c r="F12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="G12" s="1">
         <v>2017</v>
       </c>
       <c r="H12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="I12" s="1">
         <v>2017</v>
       </c>
       <c r="J12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="K12" s="1">
         <v>2017</v>
@@ -1101,19 +1101,19 @@
         <v>2022</v>
       </c>
       <c r="M12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="N12" s="1">
         <v>2022</v>
       </c>
       <c r="O12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="P12" s="1">
         <v>2022</v>
       </c>
       <c r="Q12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="R12" s="1">
         <v>2022</v>
@@ -1136,40 +1136,40 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F13" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="G13" s="1">
         <v>63.3</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
+        <v>43.5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="K13" s="1">
         <v>6.5</v>
       </c>
-      <c r="H13" s="1">
-        <v>6.2</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
       <c r="L13" s="1">
-        <v>6.7</v>
+        <v>2.9</v>
       </c>
       <c r="M13" s="1">
-        <v>43.5</v>
+        <v>0</v>
       </c>
       <c r="N13" s="1">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1">
         <v>3.3</v>
       </c>
       <c r="Q13" s="1">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
@@ -1248,40 +1248,40 @@
         <v>42.8</v>
       </c>
       <c r="F15" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="G15" s="1">
         <v>74.5</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
+        <v>61</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <v>23.2</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="L15" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>27.2</v>
-      </c>
       <c r="M15" s="1">
-        <v>61</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="O15" s="1">
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
@@ -1416,40 +1416,40 @@
         <v>32.4</v>
       </c>
       <c r="F18" s="1">
+        <v>50.4</v>
+      </c>
+      <c r="G18" s="1">
         <v>51.6</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="I18" s="1">
+        <v>88.4</v>
+      </c>
+      <c r="J18" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="K18" s="1">
         <v>53.5</v>
       </c>
-      <c r="H18" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="L18" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="M18" s="1">
         <v>113.6</v>
       </c>
-      <c r="J18" s="1">
-        <v>88.4</v>
-      </c>
-      <c r="K18" s="1">
+      <c r="N18" s="1">
+        <v>85.1</v>
+      </c>
+      <c r="O18" s="1">
         <v>338</v>
-      </c>
-      <c r="L18" s="1">
-        <v>50.4</v>
-      </c>
-      <c r="M18" s="1">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="N18" s="1">
-        <v>46.5</v>
-      </c>
-      <c r="O18" s="1">
-        <v>36.9</v>
       </c>
       <c r="P18" s="1">
         <v>380.1</v>
       </c>
       <c r="Q18" s="1">
-        <v>85.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
@@ -1472,40 +1472,40 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F19" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="G19" s="1">
         <v>54.3</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
+        <v>50.2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="J19" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="K19" s="1">
         <v>202.7</v>
       </c>
-      <c r="H19" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="L19" s="1">
+        <v>193.5</v>
+      </c>
+      <c r="M19" s="1">
         <v>525.1</v>
       </c>
-      <c r="J19" s="1">
-        <v>27.3</v>
-      </c>
-      <c r="K19" s="1">
+      <c r="N19" s="1">
+        <v>405.2</v>
+      </c>
+      <c r="O19" s="1">
         <v>15.8</v>
-      </c>
-      <c r="L19" s="1">
-        <v>30.5</v>
-      </c>
-      <c r="M19" s="1">
-        <v>50.2</v>
-      </c>
-      <c r="N19" s="1">
-        <v>15.3</v>
-      </c>
-      <c r="O19" s="1">
-        <v>193.5</v>
       </c>
       <c r="P19" s="1">
         <v>28.3</v>
       </c>
       <c r="Q19" s="1">
-        <v>405.2</v>
+        <v>3.8</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -1584,40 +1584,40 @@
         <v>92.6</v>
       </c>
       <c r="F21" s="1">
+        <v>114.8</v>
+      </c>
+      <c r="G21" s="1">
         <v>243.7</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>115.7</v>
+      </c>
+      <c r="J21" s="1">
+        <v>69.3</v>
+      </c>
+      <c r="K21" s="1">
         <v>285.89999999999998</v>
       </c>
-      <c r="H21" s="1">
-        <v>14.1</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="L21" s="1">
+        <v>237.7</v>
+      </c>
+      <c r="M21" s="1">
         <v>643.1</v>
       </c>
-      <c r="J21" s="1">
-        <v>115.7</v>
-      </c>
-      <c r="K21" s="1">
+      <c r="N21" s="1">
+        <v>495</v>
+      </c>
+      <c r="O21" s="1">
         <v>353.8</v>
-      </c>
-      <c r="L21" s="1">
-        <v>114.8</v>
-      </c>
-      <c r="M21" s="1">
-        <v>195.5</v>
-      </c>
-      <c r="N21" s="1">
-        <v>69.3</v>
-      </c>
-      <c r="O21" s="1">
-        <v>237.7</v>
       </c>
       <c r="P21" s="1">
         <v>411.7</v>
       </c>
       <c r="Q21" s="1">
-        <v>495</v>
+        <v>14.1</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C2" sqref="C2:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1712,19 +1712,19 @@
         <v>2017</v>
       </c>
       <c r="F2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="G2" s="1">
         <v>2017</v>
       </c>
       <c r="H2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="I2" s="1">
         <v>2017</v>
       </c>
       <c r="J2" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="K2" s="1">
         <v>2017</v>
@@ -1733,19 +1733,19 @@
         <v>2022</v>
       </c>
       <c r="M2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="N2" s="1">
         <v>2022</v>
       </c>
       <c r="O2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="P2" s="1">
         <v>2022</v>
       </c>
       <c r="Q2" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="R2" s="1">
         <v>2022</v>
@@ -2272,19 +2272,19 @@
         <v>2017</v>
       </c>
       <c r="F12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="G12" s="1">
         <v>2017</v>
       </c>
       <c r="H12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="I12" s="1">
         <v>2017</v>
       </c>
       <c r="J12" s="1">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="K12" s="1">
         <v>2017</v>
@@ -2293,19 +2293,19 @@
         <v>2022</v>
       </c>
       <c r="M12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="N12" s="1">
         <v>2022</v>
       </c>
       <c r="O12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="P12" s="1">
         <v>2022</v>
       </c>
       <c r="Q12" s="1">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="R12" s="1">
         <v>2022</v>

</xml_diff>